<commit_message>
Calificaciones Examen Teórico y acomodo de archivos
</commit_message>
<xml_diff>
--- a/Calificaciones.xlsx
+++ b/Calificaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugov\Documents\Tu_Nerd\Capacitación\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21840E16-DDC8-45FF-BF32-9103CAA8B668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77519084-1F45-4BFD-B4B5-02665B9146C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{71449B02-38DF-464E-9CA3-C917CB2E59AA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Nombre</t>
   </si>
@@ -57,10 +57,16 @@
     <t>Tarea 2</t>
   </si>
   <si>
-    <t>Examen</t>
-  </si>
-  <si>
     <t>Primer Módulo</t>
+  </si>
+  <si>
+    <t>Examen Practico</t>
+  </si>
+  <si>
+    <t>Examen Teórico</t>
+  </si>
+  <si>
+    <t>Tarea 3</t>
   </si>
 </sst>
 </file>
@@ -125,7 +131,43 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -248,16 +290,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84DE5DF3-200D-421E-B314-D86D8C72D661}" name="Tabla1" displayName="Tabla1" ref="A2:D6" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A2:D6" xr:uid="{84DE5DF3-200D-421E-B314-D86D8C72D661}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84DE5DF3-200D-421E-B314-D86D8C72D661}" name="Tabla1" displayName="Tabla1" ref="A2:F6" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A2:F6" xr:uid="{84DE5DF3-200D-421E-B314-D86D8C72D661}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D6">
     <sortCondition ref="A2:A6"/>
   </sortState>
-  <tableColumns count="4">
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{4B37C496-3458-4D77-A7ED-D1568EBCA99D}" name="Nombre" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{D49BDA8F-B223-4E68-BC4A-8E9CE9558421}" name="Tarea 1" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{5CF2B08D-7B38-4DC2-B02E-5F171271C6F1}" name="Tarea 2" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{B49DA4C8-7A05-4806-8065-8E517CD301CF}" name="Examen" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{B49DA4C8-7A05-4806-8065-8E517CD301CF}" name="Tarea 3" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{623C21C0-8565-49B0-AB5F-DBC793DEEF1F}" name="Examen Practico" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{D4DA89FF-3CC1-42B2-8DF3-F51DB98944B6}" name="Examen Teórico" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -560,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF0F278-D2D3-4963-8F83-DF7D98DBB50F}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,17 +615,19 @@
     <col min="1" max="1" width="46.5546875" customWidth="1"/>
     <col min="2" max="2" width="25.109375" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="29.44140625" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
+    <col min="6" max="6" width="35.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="16.8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -592,47 +638,69 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="16.8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="1">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1">
         <v>10</v>
       </c>
+      <c r="F3" s="1">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="16.8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="1">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
         <v>10</v>
       </c>
+      <c r="F4" s="1">
+        <v>3.5</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="16.8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="1">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1">
         <v>9</v>
       </c>
+      <c r="F5" s="1">
+        <v>5</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16.8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1">
         <v>9.6999999999999993</v>
+      </c>
+      <c r="F6" s="1">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calificaciones Módulos 1, 2 y 3
</commit_message>
<xml_diff>
--- a/Calificaciones.xlsx
+++ b/Calificaciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugov\Documents\Tu_Nerd\Capacitación\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugov\Documents\Tu_Nerd\Capacitación\Python Repositories\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77519084-1F45-4BFD-B4B5-02665B9146C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B280136-8C48-4B6D-B632-8D22CEE0ABDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{71449B02-38DF-464E-9CA3-C917CB2E59AA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="21">
   <si>
     <t>Nombre</t>
   </si>
@@ -67,13 +67,43 @@
   </si>
   <si>
     <t>Tarea 3</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Segundo Módulo</t>
+  </si>
+  <si>
+    <t>Tercer Módulo</t>
+  </si>
+  <si>
+    <t>Cuarto Módulo</t>
+  </si>
+  <si>
+    <t>Quinto Módulo</t>
+  </si>
+  <si>
+    <t>Examen Final</t>
+  </si>
+  <si>
+    <t>Primera Parte Teoría</t>
+  </si>
+  <si>
+    <t>Primera Parte Práctica</t>
+  </si>
+  <si>
+    <t>Seguna Parte Teoría</t>
+  </si>
+  <si>
+    <t>Segunda Parte Práctica</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +121,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Maven Pro"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -131,7 +167,565 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="39">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Maven Pro"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -290,18 +884,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84DE5DF3-200D-421E-B314-D86D8C72D661}" name="Tabla1" displayName="Tabla1" ref="A2:F6" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84DE5DF3-200D-421E-B314-D86D8C72D661}" name="Tabla1" displayName="Tabla1" ref="A2:F6" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <autoFilter ref="A2:F6" xr:uid="{84DE5DF3-200D-421E-B314-D86D8C72D661}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D6">
     <sortCondition ref="A2:A6"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{4B37C496-3458-4D77-A7ED-D1568EBCA99D}" name="Nombre" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{D49BDA8F-B223-4E68-BC4A-8E9CE9558421}" name="Tarea 1" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{5CF2B08D-7B38-4DC2-B02E-5F171271C6F1}" name="Tarea 2" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{B49DA4C8-7A05-4806-8065-8E517CD301CF}" name="Tarea 3" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{623C21C0-8565-49B0-AB5F-DBC793DEEF1F}" name="Examen Practico" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{D4DA89FF-3CC1-42B2-8DF3-F51DB98944B6}" name="Examen Teórico" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{4B37C496-3458-4D77-A7ED-D1568EBCA99D}" name="Nombre" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{D49BDA8F-B223-4E68-BC4A-8E9CE9558421}" name="Tarea 1" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{5CF2B08D-7B38-4DC2-B02E-5F171271C6F1}" name="Tarea 2" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{B49DA4C8-7A05-4806-8065-8E517CD301CF}" name="Tarea 3" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{623C21C0-8565-49B0-AB5F-DBC793DEEF1F}" name="Examen Practico" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{D4DA89FF-3CC1-42B2-8DF3-F51DB98944B6}" name="Examen Teórico" dataDxfId="31"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{584CF125-ABF5-4B79-B1E0-2EF86A89717E}" name="Tabla13" displayName="Tabla13" ref="A11:D15" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+  <autoFilter ref="A11:D15" xr:uid="{584CF125-ABF5-4B79-B1E0-2EF86A89717E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:D15">
+    <sortCondition ref="A2:A6"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{B7CFBE2B-0B8B-4898-ACC0-3B6364F55C25}" name="Nombre" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{48EF2175-8F56-4DB3-BFFE-BFD56B4B8399}" name="Tarea 1" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{53833B3E-995D-43DF-8158-63BC4C57BF72}" name="Examen Practico" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{8D8A2CE5-FFB6-4188-A77F-CEA15F70B2CE}" name="Examen Teórico" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{576AB687-1F63-40B8-A832-9C0C692749C5}" name="Tabla134" displayName="Tabla134" ref="A20:D24" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+  <autoFilter ref="A20:D24" xr:uid="{576AB687-1F63-40B8-A832-9C0C692749C5}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:B24">
+    <sortCondition ref="A2:A6"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{BF79A815-19FA-4363-8CCD-8EECEEFEE8CE}" name="Nombre" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{F684EB5C-01DC-4F4C-844E-CE793E90B9CF}" name="Tarea 1" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{BD17047B-E1CE-4E39-8BB8-5B8ABD2C8FFD}" name="Examen Practico" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{5692813E-F487-483B-B33A-52B676CB7493}" name="Examen Teórico" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C6667526-94C5-4CE4-A549-94140DFF5500}" name="Tabla1346" displayName="Tabla1346" ref="A37:D41" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A37:D41" xr:uid="{C6667526-94C5-4CE4-A549-94140DFF5500}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A38:B41">
+    <sortCondition ref="A4294967294:A2"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{CFF68DCC-EB72-4893-AA3D-8A1CC4567BDB}" name="Nombre" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{69212156-5873-458E-8C59-183E1AF86249}" name="Tarea 1" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{8085BEBF-6CCE-41D1-831B-A9F8AF0C78E4}" name="Examen Practico" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{14CA3466-783E-4312-BDC3-01DF2C8BB166}" name="Examen Teórico" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7A58911B-D845-4FAF-826A-BE7E554B94BE}" name="Tabla1347" displayName="Tabla1347" ref="A29:D33" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A29:D33" xr:uid="{7A58911B-D845-4FAF-826A-BE7E554B94BE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A30:B33">
+    <sortCondition ref="A2:A6"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{30BE241B-1413-46C7-8513-A19A62A223F7}" name="Nombre" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{907EBA6B-7539-4681-A26B-9B7D3E2AFC7A}" name="Tarea 1" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{926E0168-81C8-4299-81F1-26B7127D97A8}" name="Examen Practico" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{3379BDC2-6242-40B3-AACA-60490311FDD0}" name="Examen Teórico" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6E74FD43-8D0E-4E7B-A30F-7AFEF002C56D}" name="Tabla13468" displayName="Tabla13468" ref="A49:E53" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A49:E53" xr:uid="{6E74FD43-8D0E-4E7B-A30F-7AFEF002C56D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A50:B53">
+    <sortCondition ref="A4294967294:A2"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{377A6FF6-6B13-4D6E-ADE5-47B44C80D5C9}" name="Nombre" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{855545BA-75EA-462F-8225-02C6EAB20C90}" name="Primera Parte Teoría" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{BCA889D6-A6D9-4596-95DF-9E1ECAD41392}" name="Primera Parte Práctica" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{2505E491-0CA9-4B65-886E-8D3F2D23DB12}" name="Seguna Parte Teoría" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{9CDFCDCE-43E1-4A22-A68D-F25B5D1FE64D}" name="Segunda Parte Práctica" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -604,20 +1279,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF0F278-D2D3-4963-8F83-DF7D98DBB50F}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46.5546875" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="38.77734375" customWidth="1"/>
     <col min="5" max="5" width="32.6640625" customWidth="1"/>
-    <col min="6" max="6" width="35.5546875" customWidth="1"/>
+    <col min="6" max="6" width="40.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.8" x14ac:dyDescent="0.35">
@@ -651,9 +1326,15 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="B3" s="1">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
       <c r="E3" s="1">
         <v>10</v>
       </c>
@@ -665,9 +1346,15 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E4" s="1">
         <v>10</v>
       </c>
@@ -679,9 +1366,15 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="B5" s="1">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
       <c r="E5" s="1">
         <v>9</v>
       </c>
@@ -693,9 +1386,15 @@
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="B6" s="1">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1">
+        <v>8</v>
+      </c>
       <c r="E6" s="1">
         <v>9.6999999999999993</v>
       </c>
@@ -703,11 +1402,329 @@
         <v>9</v>
       </c>
     </row>
+    <row r="10" spans="1:6" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="28" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="36" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="48" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="1">
+        <v>4</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="1:5" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="1:5" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="1">
+        <v>7</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="6">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ejercicios de repaso: While Loop
</commit_message>
<xml_diff>
--- a/Calificaciones.xlsx
+++ b/Calificaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugov\Documents\Tu_Nerd\Capacitación\Python Repositories\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B280136-8C48-4B6D-B632-8D22CEE0ABDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D61E9EA-276F-49E4-A9EE-8610A2D6C56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{71449B02-38DF-464E-9CA3-C917CB2E59AA}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="19">
   <si>
     <t>Nombre</t>
   </si>
@@ -81,9 +82,6 @@
     <t>Cuarto Módulo</t>
   </si>
   <si>
-    <t>Quinto Módulo</t>
-  </si>
-  <si>
     <t>Examen Final</t>
   </si>
   <si>
@@ -93,10 +91,7 @@
     <t>Primera Parte Práctica</t>
   </si>
   <si>
-    <t>Seguna Parte Teoría</t>
-  </si>
-  <si>
-    <t>Segunda Parte Práctica</t>
+    <t>Segunda Parte Teoría</t>
   </si>
 </sst>
 </file>
@@ -167,133 +162,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Maven Pro"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Maven Pro"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Maven Pro"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Maven Pro"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Maven Pro"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Maven Pro"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Maven Pro"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <font>
         <b val="0"/>
@@ -884,99 +753,82 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84DE5DF3-200D-421E-B314-D86D8C72D661}" name="Tabla1" displayName="Tabla1" ref="A2:F6" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84DE5DF3-200D-421E-B314-D86D8C72D661}" name="Tabla1" displayName="Tabla1" ref="A2:F6" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A2:F6" xr:uid="{84DE5DF3-200D-421E-B314-D86D8C72D661}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D6">
     <sortCondition ref="A2:A6"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{4B37C496-3458-4D77-A7ED-D1568EBCA99D}" name="Nombre" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{D49BDA8F-B223-4E68-BC4A-8E9CE9558421}" name="Tarea 1" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{5CF2B08D-7B38-4DC2-B02E-5F171271C6F1}" name="Tarea 2" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{B49DA4C8-7A05-4806-8065-8E517CD301CF}" name="Tarea 3" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{623C21C0-8565-49B0-AB5F-DBC793DEEF1F}" name="Examen Practico" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{D4DA89FF-3CC1-42B2-8DF3-F51DB98944B6}" name="Examen Teórico" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{4B37C496-3458-4D77-A7ED-D1568EBCA99D}" name="Nombre" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{D49BDA8F-B223-4E68-BC4A-8E9CE9558421}" name="Tarea 1" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{5CF2B08D-7B38-4DC2-B02E-5F171271C6F1}" name="Tarea 2" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{B49DA4C8-7A05-4806-8065-8E517CD301CF}" name="Tarea 3" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{623C21C0-8565-49B0-AB5F-DBC793DEEF1F}" name="Examen Practico" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{D4DA89FF-3CC1-42B2-8DF3-F51DB98944B6}" name="Examen Teórico" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{584CF125-ABF5-4B79-B1E0-2EF86A89717E}" name="Tabla13" displayName="Tabla13" ref="A11:D15" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{584CF125-ABF5-4B79-B1E0-2EF86A89717E}" name="Tabla13" displayName="Tabla13" ref="A11:D15" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A11:D15" xr:uid="{584CF125-ABF5-4B79-B1E0-2EF86A89717E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:D15">
     <sortCondition ref="A2:A6"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B7CFBE2B-0B8B-4898-ACC0-3B6364F55C25}" name="Nombre" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{48EF2175-8F56-4DB3-BFFE-BFD56B4B8399}" name="Tarea 1" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{53833B3E-995D-43DF-8158-63BC4C57BF72}" name="Examen Practico" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{8D8A2CE5-FFB6-4188-A77F-CEA15F70B2CE}" name="Examen Teórico" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{B7CFBE2B-0B8B-4898-ACC0-3B6364F55C25}" name="Nombre" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{48EF2175-8F56-4DB3-BFFE-BFD56B4B8399}" name="Tarea 1" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{53833B3E-995D-43DF-8158-63BC4C57BF72}" name="Examen Practico" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{8D8A2CE5-FFB6-4188-A77F-CEA15F70B2CE}" name="Examen Teórico" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{576AB687-1F63-40B8-A832-9C0C692749C5}" name="Tabla134" displayName="Tabla134" ref="A20:D24" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{576AB687-1F63-40B8-A832-9C0C692749C5}" name="Tabla134" displayName="Tabla134" ref="A20:D24" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A20:D24" xr:uid="{576AB687-1F63-40B8-A832-9C0C692749C5}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:B24">
     <sortCondition ref="A2:A6"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BF79A815-19FA-4363-8CCD-8EECEEFEE8CE}" name="Nombre" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{F684EB5C-01DC-4F4C-844E-CE793E90B9CF}" name="Tarea 1" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{BD17047B-E1CE-4E39-8BB8-5B8ABD2C8FFD}" name="Examen Practico" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{5692813E-F487-483B-B33A-52B676CB7493}" name="Examen Teórico" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{BF79A815-19FA-4363-8CCD-8EECEEFEE8CE}" name="Nombre" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{F684EB5C-01DC-4F4C-844E-CE793E90B9CF}" name="Tarea 1" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{BD17047B-E1CE-4E39-8BB8-5B8ABD2C8FFD}" name="Examen Practico" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{5692813E-F487-483B-B33A-52B676CB7493}" name="Examen Teórico" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C6667526-94C5-4CE4-A549-94140DFF5500}" name="Tabla1346" displayName="Tabla1346" ref="A37:D41" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A37:D41" xr:uid="{C6667526-94C5-4CE4-A549-94140DFF5500}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A38:B41">
-    <sortCondition ref="A4294967294:A2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7A58911B-D845-4FAF-826A-BE7E554B94BE}" name="Tabla1347" displayName="Tabla1347" ref="A29:D33" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A29:D33" xr:uid="{7A58911B-D845-4FAF-826A-BE7E554B94BE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A30:B33">
+    <sortCondition ref="A2:A6"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CFF68DCC-EB72-4893-AA3D-8A1CC4567BDB}" name="Nombre" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{69212156-5873-458E-8C59-183E1AF86249}" name="Tarea 1" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{8085BEBF-6CCE-41D1-831B-A9F8AF0C78E4}" name="Examen Practico" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{14CA3466-783E-4312-BDC3-01DF2C8BB166}" name="Examen Teórico" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{30BE241B-1413-46C7-8513-A19A62A223F7}" name="Nombre" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{907EBA6B-7539-4681-A26B-9B7D3E2AFC7A}" name="Tarea 1" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{926E0168-81C8-4299-81F1-26B7127D97A8}" name="Examen Practico" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{3379BDC2-6242-40B3-AACA-60490311FDD0}" name="Examen Teórico" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7A58911B-D845-4FAF-826A-BE7E554B94BE}" name="Tabla1347" displayName="Tabla1347" ref="A29:D33" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A29:D33" xr:uid="{7A58911B-D845-4FAF-826A-BE7E554B94BE}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A30:B33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2B79896E-720A-4A40-BABC-93785B8F0A09}" name="Tabla13475" displayName="Tabla13475" ref="A46:D50" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A46:D50" xr:uid="{2B79896E-720A-4A40-BABC-93785B8F0A09}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A47:B50">
     <sortCondition ref="A2:A6"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{30BE241B-1413-46C7-8513-A19A62A223F7}" name="Nombre" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{907EBA6B-7539-4681-A26B-9B7D3E2AFC7A}" name="Tarea 1" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{926E0168-81C8-4299-81F1-26B7127D97A8}" name="Examen Practico" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{3379BDC2-6242-40B3-AACA-60490311FDD0}" name="Examen Teórico" dataDxfId="7"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6E74FD43-8D0E-4E7B-A30F-7AFEF002C56D}" name="Tabla13468" displayName="Tabla13468" ref="A49:E53" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A49:E53" xr:uid="{6E74FD43-8D0E-4E7B-A30F-7AFEF002C56D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A50:B53">
-    <sortCondition ref="A4294967294:A2"/>
-  </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{377A6FF6-6B13-4D6E-ADE5-47B44C80D5C9}" name="Nombre" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{855545BA-75EA-462F-8225-02C6EAB20C90}" name="Primera Parte Teoría" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{BCA889D6-A6D9-4596-95DF-9E1ECAD41392}" name="Primera Parte Práctica" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{2505E491-0CA9-4B65-886E-8D3F2D23DB12}" name="Seguna Parte Teoría" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{9CDFCDCE-43E1-4A22-A68D-F25B5D1FE64D}" name="Segunda Parte Práctica" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{2C7B4C3B-6778-4F40-A20E-5015F00AE24D}" name="Nombre" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{8C8DF5A2-F708-46DE-9B25-F955E3E20A7F}" name="Primera Parte Teoría" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{D59E8640-9320-4859-A271-744BFFB66C3C}" name="Primera Parte Práctica" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{F69695F2-C171-40C6-87B0-811D8C25AFE4}" name="Segunda Parte Teoría" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1279,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF0F278-D2D3-4963-8F83-DF7D98DBB50F}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1593,138 +1445,77 @@
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="36" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
+    <row r="45" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
+      <c r="B46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
+      <c r="B47" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-    </row>
-    <row r="48" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
-      <c r="A48" s="2" t="s">
-        <v>16</v>
+      <c r="B48" s="1">
+        <v>4</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:5" ht="16.8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="16.8" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="B49" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B50" s="1">
-        <v>7.6</v>
+        <v>7</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-    </row>
-    <row r="51" spans="1:5" ht="16.8" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B51" s="1">
-        <v>4</v>
-      </c>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-    </row>
-    <row r="52" spans="1:5" ht="16.8" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B52" s="1">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-    </row>
-    <row r="53" spans="1:5" ht="16.8" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B53" s="1">
-        <v>7</v>
-      </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="6">
+  <tableParts count="5">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
-    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>